<commit_message>
insertar texto e imagenes en seccion
</commit_message>
<xml_diff>
--- a/config/mapeo ingenieria.xlsx
+++ b/config/mapeo ingenieria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://articaingenieria-my.sharepoint.com/personal/jgarcia_articai_es/Documents/Documentos/GitHub/ing_solicitudes/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="186" documentId="11_AD4D2F04E46CFB4ACB3E208015D4F7C2693EDF1E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1D1152C-56F3-493F-8D84-50E04CAA5F0E}"/>
+  <xr:revisionPtr revIDLastSave="234" documentId="11_AD4D2F04E46CFB4ACB3E208015D4F7C2693EDF1E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4793BDAA-19E6-453F-B606-794ED9321AA6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="96">
   <si>
     <t>memoria</t>
   </si>
@@ -276,10 +276,55 @@
     <t>8. Documentos Usos Varios</t>
   </si>
   <si>
-    <t>plantilla</t>
-  </si>
-  <si>
-    <t>XXX-POOC-3. Anexo I-Memoria_TIPO</t>
+    <t>presentacion</t>
+  </si>
+  <si>
+    <t>contrato</t>
+  </si>
+  <si>
+    <t>XXX-POOC-1. Presentación_TIPO.docx</t>
+  </si>
+  <si>
+    <t>XXX-POCL-1. Presentación_TIPO.docx</t>
+  </si>
+  <si>
+    <t>XXX-POF-1. Presentación_TIPO.docx</t>
+  </si>
+  <si>
+    <t>XXX-POIF-1. Presentación_TIPO.docx</t>
+  </si>
+  <si>
+    <t>XXX-POPCI-1. Presentación_TIPO.docx</t>
+  </si>
+  <si>
+    <t>XXX-POBT-1. Presentación_TIPO.docx</t>
+  </si>
+  <si>
+    <t>XXX-POM- Pliego Maquinaria_TIPO.docx</t>
+  </si>
+  <si>
+    <t>XXX-POOC-3. Anexo I-Memoria_TIPO.docx</t>
+  </si>
+  <si>
+    <t>XXX-POOC-2. Borrador contrato_TIPO.docx</t>
+  </si>
+  <si>
+    <t>XXX-POCL-2. Borrador Contrato_TIPO.docx</t>
+  </si>
+  <si>
+    <t>XXX-POF-2. Borrador Contrato_TIPO.docx</t>
+  </si>
+  <si>
+    <t>XXX-POIF-2. Borrador Contrato_TIPO.docx</t>
+  </si>
+  <si>
+    <t>XXX-POPCI-2. Borrador Contrato_TIPO.docx</t>
+  </si>
+  <si>
+    <t>XXX-POBT-2. Borrador Contrato_TIPO.docx</t>
+  </si>
+  <si>
+    <t>proyecto</t>
   </si>
 </sst>
 </file>
@@ -401,6 +446,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -666,24 +715,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F0A5C4-EBC6-4BFC-A637-F487BCD8D1E1}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F3" sqref="F3:F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.6640625" customWidth="1"/>
-    <col min="4" max="4" width="57.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.7109375" customWidth="1"/>
+    <col min="4" max="4" width="57.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.85546875" customWidth="1"/>
+    <col min="6" max="6" width="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -697,8 +748,14 @@
       <c r="E1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -712,10 +769,16 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -729,10 +792,16 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -746,10 +815,16 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -763,10 +838,16 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -780,10 +861,16 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -797,10 +884,16 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -814,10 +907,16 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -831,10 +930,16 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -848,10 +953,16 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -865,10 +976,16 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -882,10 +999,16 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -899,10 +1022,16 @@
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -916,10 +1045,16 @@
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -933,10 +1068,16 @@
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -950,10 +1091,16 @@
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -967,10 +1114,16 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F17" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -984,10 +1137,16 @@
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1001,10 +1160,16 @@
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1018,10 +1183,16 @@
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F20" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1035,10 +1206,16 @@
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F21" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1052,10 +1229,16 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F22" t="s">
+        <v>88</v>
+      </c>
+      <c r="G22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1069,10 +1252,16 @@
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F23" t="s">
+        <v>88</v>
+      </c>
+      <c r="G23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1086,10 +1275,16 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F24" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1103,10 +1298,16 @@
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F25" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1120,10 +1321,16 @@
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F26" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1136,8 +1343,14 @@
       <c r="D27" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E27" t="s">
+        <v>82</v>
+      </c>
+      <c r="G27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1150,8 +1363,14 @@
       <c r="D28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>83</v>
+      </c>
+      <c r="G28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1164,8 +1383,14 @@
       <c r="D29" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>84</v>
+      </c>
+      <c r="G29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1178,8 +1403,14 @@
       <c r="D30" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>85</v>
+      </c>
+      <c r="G30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1192,8 +1423,14 @@
       <c r="D31" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1207,7 +1444,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -1219,6 +1456,9 @@
       </c>
       <c r="D33" t="s">
         <v>52</v>
+      </c>
+      <c r="E33" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1232,18 +1472,18 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>53</v>
       </c>
@@ -1260,14 +1500,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>58</v>
       </c>
@@ -1278,7 +1518,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="3" t="s">
         <v>60</v>
@@ -1287,7 +1527,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="3" t="s">
         <v>61</v>
@@ -1296,7 +1536,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="3" t="s">
         <v>62</v>
@@ -1305,7 +1545,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="3" t="s">
         <v>63</v>
@@ -1314,7 +1554,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="6" t="s">
         <v>64</v>
@@ -1329,7 +1569,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1338,7 +1578,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1347,7 +1587,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1356,7 +1596,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1365,7 +1605,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1374,7 +1614,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1383,7 +1623,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="6"/>
       <c r="C15" s="3" t="s">
@@ -1392,7 +1632,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="6"/>
       <c r="C16" s="3" t="s">
@@ -1401,7 +1641,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="3" t="s">
         <v>76</v>
@@ -1410,7 +1650,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="3" t="s">
         <v>77</v>
@@ -1419,7 +1659,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="3" t="s">
         <v>78</v>

</xml_diff>